<commit_message>
Update org-wide PR review report
</commit_message>
<xml_diff>
--- a/org_prs_needing_review.xlsx
+++ b/org_prs_needing_review.xlsx
@@ -397,13 +397,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="str">
+        <v>Repository</v>
+      </c>
+      <c r="B1" t="str">
+        <v>PR Number</v>
+      </c>
+      <c r="C1" t="str">
+        <v>Title</v>
+      </c>
+      <c r="D1" t="str">
+        <v>Owner</v>
+      </c>
+      <c r="E1" t="str">
+        <v>URL</v>
+      </c>
+      <c r="F1" t="str">
+        <v>Status</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>vmn_ecomm_backend</v>
+      </c>
+      <c r="B2">
+        <v>7</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Model refactoring</v>
+      </c>
+      <c r="D2" t="str">
+        <v>jaziel1974</v>
+      </c>
+      <c r="E2" t="str">
+        <v>https://github.com/jaziel1974/vmn_ecomm_backend/pull/7</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Needs Review</v>
+      </c>
+    </row>
+  </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>